<commit_message>
One click report (#3)
* Major code edit

* Initial update
</commit_message>
<xml_diff>
--- a/TraysFastUpdate/wwwroot/CableTypes.xlsx
+++ b/TraysFastUpdate/wwwroot/CableTypes.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CableTypes" sheetId="1" r:id="Rb8cb2310244442e4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CableTypes" sheetId="1" r:id="R92a6a715fd414d82"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CableTypes" displayName="CableTypes" ref="A1:D37">
-  <x:autoFilter ref="A1:D37"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CableTypes" displayName="CableTypes" ref="A1:D42">
+  <x:autoFilter ref="A1:D42"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="Type"/>
     <x:tableColumn id="2" name="Purpose"/>
@@ -541,9 +541,79 @@
         <x:v>5.305</x:v>
       </x:c>
     </x:row>
+    <x:row r="38">
+      <x:c r="A38" t="str">
+        <x:v>N2XH-Flex 0.6/1 kV 4G2.5mm²</x:v>
+      </x:c>
+      <x:c r="B38" t="str">
+        <x:v>Power</x:v>
+      </x:c>
+      <x:c r="C38" t="n">
+        <x:v>12.20</x:v>
+      </x:c>
+      <x:c r="D38" t="n">
+        <x:v>0.225</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39">
+      <x:c r="A39" t="str">
+        <x:v>N2XH-Flex 0.6/1 kV 4G25mm²</x:v>
+      </x:c>
+      <x:c r="B39" t="str">
+        <x:v>Power</x:v>
+      </x:c>
+      <x:c r="C39" t="n">
+        <x:v>23.80</x:v>
+      </x:c>
+      <x:c r="D39" t="n">
+        <x:v>1.275</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40">
+      <x:c r="A40" t="str">
+        <x:v>N2XH-Flex 0.6/1 kV 4G50mm²</x:v>
+      </x:c>
+      <x:c r="B40" t="str">
+        <x:v>Power</x:v>
+      </x:c>
+      <x:c r="C40" t="n">
+        <x:v>30.10</x:v>
+      </x:c>
+      <x:c r="D40" t="n">
+        <x:v>2.310</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41">
+      <x:c r="A41" t="str">
+        <x:v>N2XH-Flex 0.6/1 kV 4G70mm²</x:v>
+      </x:c>
+      <x:c r="B41" t="str">
+        <x:v>Power</x:v>
+      </x:c>
+      <x:c r="C41" t="n">
+        <x:v>34.80</x:v>
+      </x:c>
+      <x:c r="D41" t="n">
+        <x:v>3.185</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42">
+      <x:c r="A42" t="str">
+        <x:v>N2XH-Flex 0.6/1 kV 4G95mm²</x:v>
+      </x:c>
+      <x:c r="B42" t="str">
+        <x:v>Power</x:v>
+      </x:c>
+      <x:c r="C42" t="n">
+        <x:v>39.90</x:v>
+      </x:c>
+      <x:c r="D42" t="n">
+        <x:v>4.184</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:tableParts>
-    <x:tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R82e242db69e841be"/>
+    <x:tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R7069d7fdcbc2489b"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>